<commit_message>
Getting code clean and ordered
</commit_message>
<xml_diff>
--- a/data_to_use/merged_data/Data_Count.xlsx
+++ b/data_to_use/merged_data/Data_Count.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Thesis_AnaPao\data_to_use\merged_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E5F15C-53FF-4E70-B481-8E818E519632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B95113-B408-40BD-A2C2-00A8E18775D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">anxiety </t>
   </si>
   <si>
     <t>depression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Utilizar usuarios encontrados en 2 y comparar con paso 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Seleccionar los usuarios mas depresivos (con mas Trues que Falses, groupby(username)) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Documentar todo, elaborar graficas, sacar conclusiones y confirmar o negar hipotesis </t>
+  </si>
+  <si>
+    <t>1. Meter los datos del 2019 al classificador y ver que sale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Hacer el paso 1 y 2 con los del 2020 </t>
   </si>
 </sst>
 </file>
@@ -46,12 +61,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -81,10 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,7 +399,7 @@
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="1">
         <v>2019</v>
@@ -385,7 +408,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -395,16 +418,53 @@
       <c r="C3" s="1">
         <v>3803</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="E3">
+        <v>3089</v>
+      </c>
+      <c r="F3">
+        <v>3956</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>4998</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>4995</v>
+      </c>
+      <c r="E4">
+        <v>4995</v>
+      </c>
+      <c r="F4" s="4">
+        <v>4996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>